<commit_message>
all documents added on pdf format.
</commit_message>
<xml_diff>
--- a/Documents/Analiz-Dokümani.xlsx
+++ b/Documents/Analiz-Dokümani.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bedir\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bedir\Desktop\quest-map\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC5329FA-EA71-4CDD-8A60-4FB2D9A745C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E7E734-F91C-4F6C-BA22-754261F5D19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B2A4827E-1C31-4C3D-8DCF-C5C51CC6220A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Gereksinim No</t>
   </si>
@@ -69,30 +69,12 @@
     <t>Quest Map uygulaması Android v.5.0'dan sonrasını destekler.</t>
   </si>
   <si>
-    <t>Quest Map uygulaması bir harita uygulamasıdır. Kullanıclar bu uygulamaya Google Play Store üzerinden cihazlarına indirerek ulaşabilirler.</t>
-  </si>
-  <si>
-    <t>Uygulama açıldığında splash screen de uygulama adı ve logosu görüldükten sonra açılış ekranında kullanıcının kaydedilmiş konumları listelenir. İlk açılışta bu liste boş olacaktır</t>
-  </si>
-  <si>
-    <t>Kaydedilen konumların listelendiği ekranın sağ altında bulunan "+" butonuna basıldığında Google Maps sayfası açılır ve kullanıcının bulunduğu konum belli bir uzaklaştırma oranı ile görüntülenir</t>
-  </si>
-  <si>
-    <t>Kullancı kaydetmek istediği konum üzerine basılı tutarak açılan pencerede konumun kaydedileceği ismi klavyesinden tuşlayarak belirler.</t>
-  </si>
-  <si>
-    <t>Kaydedilmek istenen konumun ismi belirlendikten sonra "Kaydet" butonuna basarak konum kaydedilir ve başlangıç sayfasında o konum listelenir.</t>
-  </si>
-  <si>
     <t>Kullanıcılar istedikleri kadar konum ekleyip bu listede görüntüleyebilirler.</t>
   </si>
   <si>
     <t xml:space="preserve">Kaydedilen bir konuma tıklandığında o konum harita üzerinde kaydediliği ismi ile görüntülenir. </t>
   </si>
   <si>
-    <t>Kullancılar tercihlerine göre kaydettikleri konumları silebilir veya o konumlara Google Maps üzerinden yol tarifi alabilirler.</t>
-  </si>
-  <si>
     <t>G8</t>
   </si>
   <si>
@@ -102,7 +84,28 @@
     <t>G10</t>
   </si>
   <si>
-    <t>Kaydedilen konumların listelendiği ekranın sağ altında bulunan "+" butonuna basıldığında Google Maps sayfası açılır ve kullanıcının bulunduğu konum belli bir uzaklaştırma oranı ile görüntülenir.</t>
+    <t>Kaydedilen konumların listelendiği ekranın sağ altında bulunan "+" butonuna basıldığında Google Maps sayfası açılır
+ ve kullanıcının bulunduğu konum belli bir uzaklaştırma oranı ile görüntülenir.</t>
+  </si>
+  <si>
+    <t>Uygulama açıldığında splash screen de uygulama adı ve logosu görüldükten sonra açılış ekranında kullanıcının
+ kaydedilmiş konumları listelenir. İlk açılışta bu liste boş olacaktır</t>
+  </si>
+  <si>
+    <t>Kullancı kaydetmek istediği konum üzerine basılı tutarak açılan pencerede konumun kaydedileceği ismi klavyesinden
+ tuşlayarak belirler.</t>
+  </si>
+  <si>
+    <t>Quest Map uygulaması bir harita uygulamasıdır. Kullanıclar bu uygulamaya Google Play Store üzerinden cihazlarına
+ indirerek ulaşabilirler.</t>
+  </si>
+  <si>
+    <t>Kaydedilmek istenen konumun ismi belirlendikten sonra "Kaydet" butonuna basarak konum kaydedilir ve başlangıç 
+sayfasında o konum listelenir.</t>
+  </si>
+  <si>
+    <t>Kullancılar tercihlerine göre kaydettikleri konumları silebilir veya o konumlara Google Maps üzerinden yol tarifi 
+alabilirler.</t>
   </si>
 </sst>
 </file>
@@ -176,11 +179,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,101 +509,101 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="186" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="112" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
+    <row r="11" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>